<commit_message>
Reading excel and ploting the QR correctly
</commit_message>
<xml_diff>
--- a/external_info/Battery.xlsx
+++ b/external_info/Battery.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>Scanner</t>
   </si>
@@ -19,7 +19,7 @@
     <t>id_scooter</t>
   </si>
   <si>
-    <t>https'//scooters.taxify.eu/qr/850-640</t>
+    <t>https'//scooters.taxify.eu/qr/851-640</t>
   </si>
 </sst>
 </file>
@@ -313,8 +313,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2:B3" si="1">RIGHTB(A2,7)</f>
-        <v>850-640</v>
+        <f t="shared" ref="B2:B6" si="1">RIGHTB(A2,7)</f>
+        <v>851-640</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -324,16 +324,37 @@
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>850-640</v>
+        <v>851-640</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>851-640</v>
+      </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>851-640</v>
+      </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>851-640</v>
+      </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7">
@@ -358,9 +379,17 @@
       <c r="C13" s="4"/>
     </row>
     <row r="14">
+      <c r="B14" s="1" t="str">
+        <f t="shared" ref="B14:B15" si="2">RIGHTB(A14,7)</f>
+        <v/>
+      </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15">
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16">

</xml_diff>